<commit_message>
Updating Metadata for T29R11 1880
</commit_message>
<xml_diff>
--- a/data/T29R11_data.xlsx
+++ b/data/T29R11_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kara Fox\Documents\Kara GLO\RStudio\GLO_sage\Sage_GLO\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3954BAE-F5F7-4507-9C48-A7791A629E4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D1112D-926E-456C-BD75-852BFFC8DFB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-5295" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-5295" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1940Survey" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="look up" sheetId="3" r:id="rId3"/>
     <sheet name="species codes" sheetId="4" r:id="rId4"/>
     <sheet name="1940Metadata" sheetId="5" r:id="rId5"/>
+    <sheet name="1880Metadata" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -239,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4795" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4796" uniqueCount="581">
   <si>
     <t>Survey_type</t>
   </si>
@@ -1979,6 +1980,9 @@
   </si>
   <si>
     <t xml:space="preserve">Sage brush valleys and flats lie around these mountains. The timber is fir, cedar, pine and pinon on top of the high mountains, becoming all cedar and pinon as the foot is approached. It affords posts and firewood but very little saw timber. The undergrowth in the margins of the timber and outside of it, is sage, which grows very densely and usually from 3-4 ft high. </t>
+  </si>
+  <si>
+    <t>29-11-05-W was not surveyed, and will stay NA.</t>
   </si>
 </sst>
 </file>
@@ -17171,7 +17175,7 @@
   </sheetPr>
   <dimension ref="A1:AB988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
+    <sheetView topLeftCell="A243" workbookViewId="0">
       <selection activeCell="E269" sqref="E269"/>
     </sheetView>
   </sheetViews>
@@ -26038,4 +26042,25 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1727F2-C405-48C8-AF30-C566419512BE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="39" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>580</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>